<commit_message>
troubleshooting inside to hp
with all deps together, need to rethink how inside vessel table gets reshaped into hp. Also found a handful of selections that need to be reviewed manually for errors and exported CSV of those to review
</commit_message>
<xml_diff>
--- a/data_inputs/Inside_Park_Tables/JURIEN_202201_JNE_inside-outside_park_a001.xlsx
+++ b/data_inputs/Inside_Park_Tables/JURIEN_202201_JNE_inside-outside_park_a001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.mccordic.NMFS\Documents\GitHub\AMP_ves_summary\data_inputs\Inside_Park_Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nefscdata\PassiveAcoustics\DATA_ANALYSIS\VESSEL\PROPAGATION\PARKS_AUSTRALIA\PARKSAUSTRALIA_JURIEN_202201_JNE\Inside Park Tables\JURIEN_202201_JNE_alpha001\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="13128" windowHeight="6108"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="13128" windowHeight="6108"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="323">
   <si>
     <t>Filename</t>
   </si>
@@ -81,6 +81,9 @@
     <t>805830683.22105023100_sel01_S1.wav</t>
   </si>
   <si>
+    <t>22105023100</t>
+  </si>
+  <si>
     <t>S1</t>
   </si>
   <si>
@@ -552,18 +555,9 @@
     <t>805830683.220130021911_sel02_S2.wav</t>
   </si>
   <si>
-    <t>805830683.220201021853_sel01_.wav</t>
-  </si>
-  <si>
     <t>220201021853</t>
   </si>
   <si>
-    <t>805830683.220201021853_sel02_.wav</t>
-  </si>
-  <si>
-    <t>805830683.220201021853_sel03_.wav</t>
-  </si>
-  <si>
     <t>805830683.220202021844_sel01_S1.wav</t>
   </si>
   <si>
@@ -988,6 +982,15 @@
   </si>
   <si>
     <t>220310021300</t>
+  </si>
+  <si>
+    <t>805830683.220201021853_sel01_S1.wav</t>
+  </si>
+  <si>
+    <t>805830683.220201021853_sel02_S2.wav</t>
+  </si>
+  <si>
+    <t>805830683.220201021853_sel03_S3.wav</t>
   </si>
 </sst>
 </file>
@@ -1323,14 +1326,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -1393,11 +1395,11 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2">
-        <v>220105023100</v>
+      <c r="B2" t="s">
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>107.684710659556</v>
@@ -1447,13 +1449,13 @@
     </row>
     <row r="3" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>220105023100</v>
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>105.08842404094</v>
@@ -1503,13 +1505,13 @@
     </row>
     <row r="4" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>97.812500460489005</v>
@@ -1559,13 +1561,13 @@
     </row>
     <row r="5" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>104.834592362042</v>
@@ -1615,13 +1617,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>136.169434176506</v>
@@ -1671,13 +1673,13 @@
     </row>
     <row r="7" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7">
         <v>114.114236975506</v>
@@ -1727,13 +1729,13 @@
     </row>
     <row r="8" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>96.638785355026599</v>
@@ -1783,13 +1785,13 @@
     </row>
     <row r="9" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9">
         <v>97.805459863688398</v>
@@ -1839,13 +1841,13 @@
     </row>
     <row r="10" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>106.181715918715</v>
@@ -1895,13 +1897,13 @@
     </row>
     <row r="11" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>104.398565318685</v>
@@ -1951,13 +1953,13 @@
     </row>
     <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>107.62979465339799</v>
@@ -2007,13 +2009,13 @@
     </row>
     <row r="13" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13">
         <v>115.55432623193001</v>
@@ -2063,13 +2065,13 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14">
         <v>138.193770523372</v>
@@ -2119,13 +2121,13 @@
     </row>
     <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15">
         <v>100.694073035386</v>
@@ -2175,13 +2177,13 @@
     </row>
     <row r="16" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>105.620814625477</v>
@@ -2231,13 +2233,13 @@
     </row>
     <row r="17" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17">
         <v>104.879125730453</v>
@@ -2287,13 +2289,13 @@
     </row>
     <row r="18" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18">
         <v>109.998241560091</v>
@@ -2343,13 +2345,13 @@
     </row>
     <row r="19" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19">
         <v>103.855119449133</v>
@@ -2399,13 +2401,13 @@
     </row>
     <row r="20" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D20">
         <v>99.192024398739903</v>
@@ -2455,13 +2457,13 @@
     </row>
     <row r="21" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D21">
         <v>102.941002540201</v>
@@ -2511,13 +2513,13 @@
     </row>
     <row r="22" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22">
         <v>101.42658004875101</v>
@@ -2567,13 +2569,13 @@
     </row>
     <row r="23" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23">
         <v>98.827856806562394</v>
@@ -2623,13 +2625,13 @@
     </row>
     <row r="24" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D24">
         <v>95.836705667641198</v>
@@ -2679,13 +2681,13 @@
     </row>
     <row r="25" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D25">
         <v>105.463813560867</v>
@@ -2735,13 +2737,13 @@
     </row>
     <row r="26" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26">
         <v>98.332314121199303</v>
@@ -2791,13 +2793,13 @@
     </row>
     <row r="27" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27">
         <v>96.503595970923797</v>
@@ -2847,13 +2849,13 @@
     </row>
     <row r="28" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D28">
         <v>97.9130182398833</v>
@@ -2903,13 +2905,13 @@
     </row>
     <row r="29" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D29">
         <v>101.2526699851</v>
@@ -2959,13 +2961,13 @@
     </row>
     <row r="30" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D30">
         <v>97.325170655037894</v>
@@ -3015,13 +3017,13 @@
     </row>
     <row r="31" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D31">
         <v>110.10221243948401</v>
@@ -3071,13 +3073,13 @@
     </row>
     <row r="32" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D32">
         <v>98.190608092312701</v>
@@ -3127,13 +3129,13 @@
     </row>
     <row r="33" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
-        <v>65</v>
-      </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D33">
         <v>98.369195678439596</v>
@@ -3183,13 +3185,13 @@
     </row>
     <row r="34" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34">
         <v>98.099044650714205</v>
@@ -3239,13 +3241,13 @@
     </row>
     <row r="35" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
         <v>69</v>
       </c>
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D35">
         <v>98.364288151133096</v>
@@ -3295,13 +3297,13 @@
     </row>
     <row r="36" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D36">
         <v>100.455941881991</v>
@@ -3351,13 +3353,13 @@
     </row>
     <row r="37" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D37">
         <v>104.10417754762599</v>
@@ -3407,13 +3409,13 @@
     </row>
     <row r="38" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D38">
         <v>99.145062102927199</v>
@@ -3463,13 +3465,13 @@
     </row>
     <row r="39" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D39">
         <v>98.158501946780305</v>
@@ -3519,13 +3521,13 @@
     </row>
     <row r="40" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D40">
         <v>102.877614788374</v>
@@ -3575,13 +3577,13 @@
     </row>
     <row r="41" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D41">
         <v>102.33184465284999</v>
@@ -3631,13 +3633,13 @@
     </row>
     <row r="42" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D42">
         <v>103.843574374577</v>
@@ -3687,13 +3689,13 @@
     </row>
     <row r="43" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>99.743356912825206</v>
@@ -3743,13 +3745,13 @@
     </row>
     <row r="44" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
         <v>80</v>
       </c>
-      <c r="B44" t="s">
-        <v>79</v>
-      </c>
       <c r="C44" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D44">
         <v>100.691423735424</v>
@@ -3799,13 +3801,13 @@
     </row>
     <row r="45" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D45">
         <v>100.047550726721</v>
@@ -3855,13 +3857,13 @@
     </row>
     <row r="46" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
         <v>83</v>
       </c>
-      <c r="B46" t="s">
-        <v>82</v>
-      </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D46">
         <v>106.465566823009</v>
@@ -3911,13 +3913,13 @@
     </row>
     <row r="47" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D47">
         <v>106.83277111089799</v>
@@ -3967,13 +3969,13 @@
     </row>
     <row r="48" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D48">
         <v>96.819717019461507</v>
@@ -4023,13 +4025,13 @@
     </row>
     <row r="49" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D49">
         <v>95.959339514835506</v>
@@ -4079,13 +4081,13 @@
     </row>
     <row r="50" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D50">
         <v>95.001154687679204</v>
@@ -4135,13 +4137,13 @@
     </row>
     <row r="51" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" t="s">
         <v>89</v>
       </c>
-      <c r="B51" t="s">
-        <v>88</v>
-      </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D51">
         <v>95.128710601993902</v>
@@ -4156,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51">
         <v>108</v>
@@ -4191,13 +4193,13 @@
     </row>
     <row r="52" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D52">
         <v>95.200151822316002</v>
@@ -4247,13 +4249,13 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D53">
         <v>139.502412868627</v>
@@ -4303,13 +4305,13 @@
     </row>
     <row r="54" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C54" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D54">
         <v>91.701367760891202</v>
@@ -4359,13 +4361,13 @@
     </row>
     <row r="55" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D55">
         <v>98.639116851001305</v>
@@ -4415,13 +4417,13 @@
     </row>
     <row r="56" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D56">
         <v>87.153890094096198</v>
@@ -4471,13 +4473,13 @@
     </row>
     <row r="57" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" t="s">
         <v>96</v>
       </c>
-      <c r="B57" t="s">
-        <v>95</v>
-      </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D57">
         <v>87.115177819108794</v>
@@ -4527,13 +4529,13 @@
     </row>
     <row r="58" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D58">
         <v>89.639519036331606</v>
@@ -4583,13 +4585,13 @@
     </row>
     <row r="59" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C59" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D59">
         <v>91.741536244178306</v>
@@ -4639,13 +4641,13 @@
     </row>
     <row r="60" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D60">
         <v>93.480264624509701</v>
@@ -4695,13 +4697,13 @@
     </row>
     <row r="61" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D61">
         <v>90.956961631922795</v>
@@ -4751,13 +4753,13 @@
     </row>
     <row r="62" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D62">
         <v>94.705596591184005</v>
@@ -4807,13 +4809,13 @@
     </row>
     <row r="63" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D63">
         <v>108.554585769491</v>
@@ -4863,13 +4865,13 @@
     </row>
     <row r="64" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D64">
         <v>102.592853044352</v>
@@ -4919,13 +4921,13 @@
     </row>
     <row r="65" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D65">
         <v>92.527616034701794</v>
@@ -4975,13 +4977,13 @@
     </row>
     <row r="66" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" t="s">
         <v>106</v>
       </c>
-      <c r="B66" t="s">
-        <v>105</v>
-      </c>
       <c r="C66" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D66">
         <v>109.53265334568199</v>
@@ -5031,13 +5033,13 @@
     </row>
     <row r="67" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D67">
         <v>101.934974673566</v>
@@ -5087,13 +5089,13 @@
     </row>
     <row r="68" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" t="s">
         <v>109</v>
       </c>
-      <c r="B68" t="s">
-        <v>108</v>
-      </c>
       <c r="C68" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D68">
         <v>92.858879085035596</v>
@@ -5143,13 +5145,13 @@
     </row>
     <row r="69" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D69">
         <v>90.861304905436</v>
@@ -5199,13 +5201,13 @@
     </row>
     <row r="70" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C70" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D70">
         <v>98.896325300498404</v>
@@ -5255,13 +5257,13 @@
     </row>
     <row r="71" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" t="s">
         <v>113</v>
       </c>
-      <c r="B71" t="s">
-        <v>112</v>
-      </c>
       <c r="C71" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D71">
         <v>93.876617773020897</v>
@@ -5311,13 +5313,13 @@
     </row>
     <row r="72" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C72" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D72">
         <v>124.903718884706</v>
@@ -5367,13 +5369,13 @@
     </row>
     <row r="73" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B73" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D73">
         <v>99.477956258186893</v>
@@ -5423,13 +5425,13 @@
     </row>
     <row r="74" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D74">
         <v>90.726370136622293</v>
@@ -5479,13 +5481,13 @@
     </row>
     <row r="75" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C75" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D75">
         <v>95.7357989236951</v>
@@ -5535,13 +5537,13 @@
     </row>
     <row r="76" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D76">
         <v>88.533324767183203</v>
@@ -5591,13 +5593,13 @@
     </row>
     <row r="77" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D77">
         <v>118.157573207513</v>
@@ -5647,13 +5649,13 @@
     </row>
     <row r="78" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" t="s">
         <v>121</v>
       </c>
-      <c r="B78" t="s">
-        <v>120</v>
-      </c>
       <c r="C78" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D78">
         <v>91.496207648871106</v>
@@ -5703,13 +5705,13 @@
     </row>
     <row r="79" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C79" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D79">
         <v>88.223269706279495</v>
@@ -5759,13 +5761,13 @@
     </row>
     <row r="80" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B80" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C80" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D80">
         <v>89.268165548699699</v>
@@ -5815,13 +5817,13 @@
     </row>
     <row r="81" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B81" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C81" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D81">
         <v>98.031166624645394</v>
@@ -5871,13 +5873,13 @@
     </row>
     <row r="82" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B82" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C82" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D82">
         <v>94.762666786813298</v>
@@ -5927,13 +5929,13 @@
     </row>
     <row r="83" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D83">
         <v>91.199766336562405</v>
@@ -5983,13 +5985,13 @@
     </row>
     <row r="84" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B84" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C84" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D84">
         <v>93.256252623683295</v>
@@ -6039,13 +6041,13 @@
     </row>
     <row r="85" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C85" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D85">
         <v>104.54831620793099</v>
@@ -6095,13 +6097,13 @@
     </row>
     <row r="86" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B86" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C86" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D86">
         <v>104.52064820653401</v>
@@ -6151,13 +6153,13 @@
     </row>
     <row r="87" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B87" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C87" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D87">
         <v>101.752618873481</v>
@@ -6207,13 +6209,13 @@
     </row>
     <row r="88" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" t="s">
         <v>134</v>
       </c>
-      <c r="B88" t="s">
-        <v>133</v>
-      </c>
       <c r="C88" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D88">
         <v>112.407656279699</v>
@@ -6263,13 +6265,13 @@
     </row>
     <row r="89" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B89" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C89" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D89">
         <v>100.748884661215</v>
@@ -6319,13 +6321,13 @@
     </row>
     <row r="90" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>138</v>
+      </c>
+      <c r="B90" t="s">
         <v>137</v>
       </c>
-      <c r="B90" t="s">
-        <v>136</v>
-      </c>
       <c r="C90" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D90">
         <v>101.59664346265799</v>
@@ -6375,13 +6377,13 @@
     </row>
     <row r="91" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B91" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C91" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D91">
         <v>104.81215702070701</v>
@@ -6431,13 +6433,13 @@
     </row>
     <row r="92" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" t="s">
         <v>140</v>
       </c>
-      <c r="B92" t="s">
-        <v>139</v>
-      </c>
       <c r="C92" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D92">
         <v>94.868200721909403</v>
@@ -6487,13 +6489,13 @@
     </row>
     <row r="93" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B93" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C93" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D93">
         <v>103.57281032433799</v>
@@ -6543,13 +6545,13 @@
     </row>
     <row r="94" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B94" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C94" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D94">
         <v>113.58981138828</v>
@@ -6599,13 +6601,13 @@
     </row>
     <row r="95" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B95" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C95" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D95">
         <v>102.60976945767101</v>
@@ -6655,13 +6657,13 @@
     </row>
     <row r="96" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B96" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C96" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D96">
         <v>111.600595567177</v>
@@ -6711,13 +6713,13 @@
     </row>
     <row r="97" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B97" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C97" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D97">
         <v>102.413648869735</v>
@@ -6767,13 +6769,13 @@
     </row>
     <row r="98" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B98" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C98" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D98">
         <v>100.766653348847</v>
@@ -6823,13 +6825,13 @@
     </row>
     <row r="99" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>149</v>
+      </c>
+      <c r="B99" t="s">
         <v>148</v>
       </c>
-      <c r="B99" t="s">
-        <v>147</v>
-      </c>
       <c r="C99" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D99">
         <v>100.564724466394</v>
@@ -6879,13 +6881,13 @@
     </row>
     <row r="100" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B100" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C100" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D100">
         <v>121.826480567386</v>
@@ -6935,13 +6937,13 @@
     </row>
     <row r="101" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B101" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D101">
         <v>116.533559864927</v>
@@ -6991,13 +6993,13 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B102" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C102" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D102">
         <v>129.20323615682199</v>
@@ -7047,13 +7049,13 @@
     </row>
     <row r="103" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B103" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C103" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D103">
         <v>97.555620495263597</v>
@@ -7068,7 +7070,7 @@
         <v>1</v>
       </c>
       <c r="H103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103">
         <v>226</v>
@@ -7103,13 +7105,13 @@
     </row>
     <row r="104" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>156</v>
+      </c>
+      <c r="B104" t="s">
         <v>155</v>
       </c>
-      <c r="B104" t="s">
-        <v>154</v>
-      </c>
       <c r="C104" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D104">
         <v>98.281610736329299</v>
@@ -7124,7 +7126,7 @@
         <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104">
         <v>206</v>
@@ -7159,13 +7161,13 @@
     </row>
     <row r="105" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B105" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C105" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D105">
         <v>97.931331025306307</v>
@@ -7215,13 +7217,13 @@
     </row>
     <row r="106" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B106" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C106" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D106">
         <v>97.318431084988802</v>
@@ -7271,13 +7273,13 @@
     </row>
     <row r="107" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B107" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C107" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D107">
         <v>98.079175546812493</v>
@@ -7327,13 +7329,13 @@
     </row>
     <row r="108" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B108" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C108" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D108">
         <v>113.822611883921</v>
@@ -7383,13 +7385,13 @@
     </row>
     <row r="109" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B109" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C109" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D109">
         <v>109.961144884779</v>
@@ -7439,13 +7441,13 @@
     </row>
     <row r="110" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B110" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C110" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D110">
         <v>94.288201821137804</v>
@@ -7495,13 +7497,13 @@
     </row>
     <row r="111" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B111" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C111" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D111">
         <v>93.034361748391802</v>
@@ -7551,13 +7553,13 @@
     </row>
     <row r="112" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B112" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C112" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D112">
         <v>90.298008111571406</v>
@@ -7607,13 +7609,13 @@
     </row>
     <row r="113" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B113" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C113" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D113">
         <v>91.494405430666902</v>
@@ -7663,13 +7665,13 @@
     </row>
     <row r="114" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B114" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C114" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D114">
         <v>97.936760924323806</v>
@@ -7719,13 +7721,13 @@
     </row>
     <row r="115" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B115" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C115" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D115">
         <v>88.952072353835504</v>
@@ -7775,13 +7777,13 @@
     </row>
     <row r="116" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>169</v>
+      </c>
+      <c r="B116" t="s">
         <v>168</v>
       </c>
-      <c r="B116" t="s">
-        <v>167</v>
-      </c>
       <c r="C116" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D116">
         <v>91.358841379845202</v>
@@ -7831,13 +7833,13 @@
     </row>
     <row r="117" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B117" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C117" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D117">
         <v>119.082977814637</v>
@@ -7887,13 +7889,13 @@
     </row>
     <row r="118" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B118" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D118">
         <v>116.155263247354</v>
@@ -7943,13 +7945,13 @@
     </row>
     <row r="119" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B119" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C119" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D119">
         <v>110.153891165524</v>
@@ -7999,13 +8001,13 @@
     </row>
     <row r="120" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B120" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C120" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D120">
         <v>102.654410262962</v>
@@ -8055,13 +8057,13 @@
     </row>
     <row r="121" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B121" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C121" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D121">
         <v>97.8439077951748</v>
@@ -8111,13 +8113,13 @@
     </row>
     <row r="122" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>176</v>
+      </c>
+      <c r="B122" t="s">
         <v>175</v>
       </c>
-      <c r="B122" t="s">
-        <v>174</v>
-      </c>
       <c r="C122" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D122">
         <v>105.01530184047</v>
@@ -8167,11 +8169,14 @@
     </row>
     <row r="123" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>176</v>
+        <v>320</v>
       </c>
       <c r="B123" t="s">
         <v>177</v>
       </c>
+      <c r="C123" t="s">
+        <v>20</v>
+      </c>
       <c r="D123">
         <v>108.51528956238199</v>
       </c>
@@ -8220,11 +8225,14 @@
     </row>
     <row r="124" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>178</v>
+        <v>321</v>
       </c>
       <c r="B124" t="s">
         <v>177</v>
       </c>
+      <c r="C124" t="s">
+        <v>25</v>
+      </c>
       <c r="D124">
         <v>99.252568050981196</v>
       </c>
@@ -8273,11 +8281,14 @@
     </row>
     <row r="125" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
       <c r="B125" t="s">
         <v>177</v>
       </c>
+      <c r="C125" t="s">
+        <v>30</v>
+      </c>
       <c r="D125">
         <v>108.77172207942399</v>
       </c>
@@ -8326,13 +8337,13 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B126" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C126" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D126">
         <v>128.793531766336</v>
@@ -8382,13 +8393,13 @@
     </row>
     <row r="127" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B127" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C127" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D127">
         <v>98.500384894102893</v>
@@ -8438,13 +8449,13 @@
     </row>
     <row r="128" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B128" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C128" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D128">
         <v>98.828569765538404</v>
@@ -8494,13 +8505,13 @@
     </row>
     <row r="129" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B129" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C129" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D129">
         <v>92.518189037094999</v>
@@ -8550,13 +8561,13 @@
     </row>
     <row r="130" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B130" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C130" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D130">
         <v>93.751321599315801</v>
@@ -8571,7 +8582,7 @@
         <v>1</v>
       </c>
       <c r="H130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I130">
         <v>156</v>
@@ -8606,13 +8617,13 @@
     </row>
     <row r="131" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B131" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C131" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D131">
         <v>93.946279069735397</v>
@@ -8662,13 +8673,13 @@
     </row>
     <row r="132" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B132" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C132" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D132">
         <v>96.378724002419403</v>
@@ -8718,13 +8729,13 @@
     </row>
     <row r="133" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B133" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C133" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D133">
         <v>100.720469586286</v>
@@ -8739,7 +8750,7 @@
         <v>1</v>
       </c>
       <c r="H133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I133">
         <v>249</v>
@@ -8774,13 +8785,13 @@
     </row>
     <row r="134" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B134" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C134" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D134">
         <v>101.596082356964</v>
@@ -8830,13 +8841,13 @@
     </row>
     <row r="135" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B135" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C135" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D135">
         <v>104.639410166239</v>
@@ -8851,7 +8862,7 @@
         <v>1</v>
       </c>
       <c r="H135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I135">
         <v>267</v>
@@ -8886,13 +8897,13 @@
     </row>
     <row r="136" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B136" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C136" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D136">
         <v>90.904145918282396</v>
@@ -8907,7 +8918,7 @@
         <v>1</v>
       </c>
       <c r="H136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I136">
         <v>104</v>
@@ -8942,13 +8953,13 @@
     </row>
     <row r="137" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B137" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C137" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D137">
         <v>92.796746410117294</v>
@@ -8998,13 +9009,13 @@
     </row>
     <row r="138" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B138" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C138" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D138">
         <v>87.461294858070403</v>
@@ -9054,13 +9065,13 @@
     </row>
     <row r="139" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B139" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C139" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D139">
         <v>99.795281895587806</v>
@@ -9110,13 +9121,13 @@
     </row>
     <row r="140" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B140" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C140" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D140">
         <v>87.157770925777697</v>
@@ -9166,13 +9177,13 @@
     </row>
     <row r="141" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B141" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C141" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D141">
         <v>92.633016173650901</v>
@@ -9222,13 +9233,13 @@
     </row>
     <row r="142" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B142" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C142" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D142">
         <v>120.33819309474499</v>
@@ -9278,13 +9289,13 @@
     </row>
     <row r="143" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B143" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C143" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D143">
         <v>107.560379879352</v>
@@ -9334,13 +9345,13 @@
     </row>
     <row r="144" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B144" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C144" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D144">
         <v>106.589872456386</v>
@@ -9390,13 +9401,13 @@
     </row>
     <row r="145" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B145" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C145" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D145">
         <v>105.244111579674</v>
@@ -9446,13 +9457,13 @@
     </row>
     <row r="146" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B146" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C146" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D146">
         <v>93.487365490645104</v>
@@ -9502,13 +9513,13 @@
     </row>
     <row r="147" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B147" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C147" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D147">
         <v>95.357876031165105</v>
@@ -9558,13 +9569,13 @@
     </row>
     <row r="148" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B148" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C148" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D148">
         <v>85.400692209617105</v>
@@ -9614,13 +9625,13 @@
     </row>
     <row r="149" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B149" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C149" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D149">
         <v>84.763691281936801</v>
@@ -9670,13 +9681,13 @@
     </row>
     <row r="150" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B150" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C150" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D150">
         <v>89.228564019372499</v>
@@ -9726,13 +9737,13 @@
     </row>
     <row r="151" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B151" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C151" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D151">
         <v>104.698679696136</v>
@@ -9782,13 +9793,13 @@
     </row>
     <row r="152" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B152" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C152" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D152">
         <v>91.292429151947701</v>
@@ -9838,13 +9849,13 @@
     </row>
     <row r="153" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B153" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C153" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D153">
         <v>90.662246069155302</v>
@@ -9894,13 +9905,13 @@
     </row>
     <row r="154" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B154" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C154" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D154">
         <v>89.308892629842205</v>
@@ -9950,13 +9961,13 @@
     </row>
     <row r="155" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B155" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C155" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D155">
         <v>92.094173960763399</v>
@@ -10006,13 +10017,13 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B156" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C156" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D156">
         <v>132.81473234084001</v>
@@ -10062,13 +10073,13 @@
     </row>
     <row r="157" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B157" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C157" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D157">
         <v>96.326766375054007</v>
@@ -10118,13 +10129,13 @@
     </row>
     <row r="158" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B158" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C158" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D158">
         <v>94.943645382897998</v>
@@ -10174,13 +10185,13 @@
     </row>
     <row r="159" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B159" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C159" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D159">
         <v>96.540182242225299</v>
@@ -10230,13 +10241,13 @@
     </row>
     <row r="160" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C160" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D160">
         <v>105.048563949543</v>
@@ -10286,13 +10297,13 @@
     </row>
     <row r="161" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B161" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C161" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D161">
         <v>116.517841369002</v>
@@ -10342,13 +10353,13 @@
     </row>
     <row r="162" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B162" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C162" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D162">
         <v>109.291547129111</v>
@@ -10398,13 +10409,13 @@
     </row>
     <row r="163" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B163" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C163" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D163">
         <v>123.626551564501</v>
@@ -10454,13 +10465,13 @@
     </row>
     <row r="164" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B164" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C164" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D164">
         <v>103.01743548156</v>
@@ -10510,13 +10521,13 @@
     </row>
     <row r="165" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B165" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C165" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D165">
         <v>106.689002251993</v>
@@ -10566,13 +10577,13 @@
     </row>
     <row r="166" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B166" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C166" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D166">
         <v>108.816857755467</v>
@@ -10622,13 +10633,13 @@
     </row>
     <row r="167" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B167" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C167" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D167">
         <v>101.220791594166</v>
@@ -10678,13 +10689,13 @@
     </row>
     <row r="168" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B168" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C168" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D168">
         <v>97.783398043005107</v>
@@ -10734,13 +10745,13 @@
     </row>
     <row r="169" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B169" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C169" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D169">
         <v>102.091548824266</v>
@@ -10790,13 +10801,13 @@
     </row>
     <row r="170" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B170" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C170" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D170">
         <v>104.032078692037</v>
@@ -10846,13 +10857,13 @@
     </row>
     <row r="171" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B171" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C171" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D171">
         <v>95.713987743801297</v>
@@ -10902,13 +10913,13 @@
     </row>
     <row r="172" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B172" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C172" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D172">
         <v>98.355508689273705</v>
@@ -10958,13 +10969,13 @@
     </row>
     <row r="173" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B173" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C173" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D173">
         <v>87.138524032293503</v>
@@ -11014,13 +11025,13 @@
     </row>
     <row r="174" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B174" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C174" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D174">
         <v>100.846536881544</v>
@@ -11070,13 +11081,13 @@
     </row>
     <row r="175" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B175" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C175" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D175">
         <v>98.4302752457195</v>
@@ -11126,13 +11137,13 @@
     </row>
     <row r="176" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B176" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C176" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D176">
         <v>98.599824637966293</v>
@@ -11182,13 +11193,13 @@
     </row>
     <row r="177" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B177" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C177" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D177">
         <v>102.278111105943</v>
@@ -11238,13 +11249,13 @@
     </row>
     <row r="178" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B178" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C178" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D178">
         <v>99.979984031507399</v>
@@ -11294,13 +11305,13 @@
     </row>
     <row r="179" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B179" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C179" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D179">
         <v>121.55665246309999</v>
@@ -11350,13 +11361,13 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B180" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C180" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D180">
         <v>128.74766136552</v>
@@ -11406,13 +11417,13 @@
     </row>
     <row r="181" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B181" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C181" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D181">
         <v>97.171774034972501</v>
@@ -11462,13 +11473,13 @@
     </row>
     <row r="182" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B182" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C182" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D182">
         <v>102.186687513127</v>
@@ -11518,13 +11529,13 @@
     </row>
     <row r="183" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B183" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C183" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D183">
         <v>100.22912276828001</v>
@@ -11574,13 +11585,13 @@
     </row>
     <row r="184" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B184" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C184" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D184">
         <v>105.909069011941</v>
@@ -11630,13 +11641,13 @@
     </row>
     <row r="185" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B185" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C185" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D185">
         <v>89.576473501429007</v>
@@ -11686,13 +11697,13 @@
     </row>
     <row r="186" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B186" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C186" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D186">
         <v>103.442557917926</v>
@@ -11742,13 +11753,13 @@
     </row>
     <row r="187" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B187" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C187" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D187">
         <v>88.735213458492893</v>
@@ -11798,13 +11809,13 @@
     </row>
     <row r="188" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B188" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C188" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D188">
         <v>87.434290998293903</v>
@@ -11854,13 +11865,13 @@
     </row>
     <row r="189" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B189" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C189" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D189">
         <v>89.191715374339495</v>
@@ -11910,13 +11921,13 @@
     </row>
     <row r="190" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B190" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C190" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D190">
         <v>89.405895457775401</v>
@@ -11966,13 +11977,13 @@
     </row>
     <row r="191" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B191" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C191" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D191">
         <v>104.64605848340901</v>
@@ -12022,13 +12033,13 @@
     </row>
     <row r="192" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B192" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C192" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D192">
         <v>97.120929785821502</v>
@@ -12078,13 +12089,13 @@
     </row>
     <row r="193" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B193" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C193" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D193">
         <v>94.843877563373297</v>
@@ -12134,13 +12145,13 @@
     </row>
     <row r="194" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B194" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C194" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D194">
         <v>98.680203670792096</v>
@@ -12190,13 +12201,13 @@
     </row>
     <row r="195" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B195" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C195" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D195">
         <v>114.589403340022</v>
@@ -12246,13 +12257,13 @@
     </row>
     <row r="196" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B196" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C196" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D196">
         <v>96.085773662185105</v>
@@ -12302,13 +12313,13 @@
     </row>
     <row r="197" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B197" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C197" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D197">
         <v>95.073366962465997</v>
@@ -12358,13 +12369,13 @@
     </row>
     <row r="198" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B198" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C198" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D198">
         <v>106.729739254962</v>
@@ -12414,13 +12425,13 @@
     </row>
     <row r="199" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B199" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C199" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D199">
         <v>106.40275866069901</v>
@@ -12470,13 +12481,13 @@
     </row>
     <row r="200" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B200" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C200" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D200">
         <v>98.348743877865104</v>
@@ -12526,13 +12537,13 @@
     </row>
     <row r="201" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B201" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C201" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D201">
         <v>96.742271100920107</v>
@@ -12582,13 +12593,13 @@
     </row>
     <row r="202" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B202" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C202" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D202">
         <v>98.963422739870595</v>
@@ -12638,13 +12649,13 @@
     </row>
     <row r="203" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B203" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C203" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D203">
         <v>100.001096802234</v>
@@ -12694,13 +12705,13 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B204" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C204" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D204">
         <v>125.832317880785</v>
@@ -12750,13 +12761,13 @@
     </row>
     <row r="205" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B205" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C205" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D205">
         <v>92.381446639601407</v>
@@ -12806,13 +12817,13 @@
     </row>
     <row r="206" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B206" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C206" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D206">
         <v>92.633075837532999</v>
@@ -12862,13 +12873,13 @@
     </row>
     <row r="207" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B207" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C207" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D207">
         <v>96.612977194442493</v>
@@ -12918,13 +12929,13 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B208" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C208" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D208">
         <v>138.41931405181199</v>
@@ -12974,13 +12985,13 @@
     </row>
     <row r="209" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B209" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C209" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D209">
         <v>97.787233661791106</v>
@@ -13030,13 +13041,13 @@
     </row>
     <row r="210" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B210" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C210" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D210">
         <v>108.312164816208</v>
@@ -13086,13 +13097,13 @@
     </row>
     <row r="211" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B211" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C211" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D211">
         <v>100.775486516261</v>
@@ -13142,13 +13153,13 @@
     </row>
     <row r="212" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B212" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C212" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D212">
         <v>110.292390425706</v>
@@ -13198,13 +13209,13 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B213" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C213" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D213">
         <v>125.69167222989699</v>
@@ -13254,13 +13265,13 @@
     </row>
     <row r="214" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B214" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C214" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D214">
         <v>91.954496371710704</v>
@@ -13310,13 +13321,13 @@
     </row>
     <row r="215" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B215" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C215" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D215">
         <v>112.384504054582</v>
@@ -13366,13 +13377,13 @@
     </row>
     <row r="216" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B216" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C216" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D216">
         <v>101.988348193801</v>
@@ -13422,13 +13433,13 @@
     </row>
     <row r="217" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B217" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C217" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D217">
         <v>109.293850045071</v>
@@ -13478,13 +13489,13 @@
     </row>
     <row r="218" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B218" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C218" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D218">
         <v>97.976493157139799</v>
@@ -13534,13 +13545,13 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B219" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C219" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D219">
         <v>127.567999000283</v>
@@ -13590,13 +13601,13 @@
     </row>
     <row r="220" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B220" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C220" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D220">
         <v>99.204236565336601</v>
@@ -13646,13 +13657,13 @@
     </row>
     <row r="221" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B221" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C221" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D221">
         <v>91.405799322782698</v>
@@ -13702,13 +13713,13 @@
     </row>
     <row r="222" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B222" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C222" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D222">
         <v>91.639156803248994</v>
@@ -13758,13 +13769,13 @@
     </row>
     <row r="223" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B223" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C223" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D223">
         <v>86.002074859483798</v>
@@ -13814,13 +13825,13 @@
     </row>
     <row r="224" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B224" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C224" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D224">
         <v>90.474968107636798</v>
@@ -13870,13 +13881,13 @@
     </row>
     <row r="225" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B225" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C225" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D225">
         <v>87.315857936749893</v>
@@ -13926,13 +13937,13 @@
     </row>
     <row r="226" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B226" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C226" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D226">
         <v>89.238117274985598</v>
@@ -13982,13 +13993,13 @@
     </row>
     <row r="227" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B227" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C227" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D227">
         <v>87.355016847569701</v>
@@ -14038,13 +14049,13 @@
     </row>
     <row r="228" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B228" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C228" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D228">
         <v>98.232724638928303</v>
@@ -14094,13 +14105,13 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B229" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C229" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D229">
         <v>133.40774569152501</v>
@@ -14150,13 +14161,13 @@
     </row>
     <row r="230" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B230" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C230" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D230">
         <v>101.32091584539</v>
@@ -14206,13 +14217,13 @@
     </row>
     <row r="231" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B231" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C231" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D231">
         <v>102.305557118956</v>
@@ -14262,13 +14273,13 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B232" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C232" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D232">
         <v>127.120542050053</v>
@@ -14318,13 +14329,13 @@
     </row>
     <row r="233" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B233" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C233" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D233">
         <v>100.717069492777</v>
@@ -14374,13 +14385,13 @@
     </row>
     <row r="234" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B234" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C234" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D234">
         <v>97.293014250159999</v>
@@ -14430,13 +14441,13 @@
     </row>
     <row r="235" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B235" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C235" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D235">
         <v>117.61871761208199</v>

</xml_diff>